<commit_message>
Update discovery questionnaire with enhanced template-based converter
- Regenerated using new convert_discovery_questionnaire.py
- File size: 11KB -> 140KB (13x larger)
- Sheets: 1 -> 12 (Cover + All Categories + 10 category sheets)
- Features: Branded template, professional styling, formulas, read-only protection
- Generated with eof-tools converter v1.0 (2025-11-19)

Old: Blank workbook with single sheet
New: Professional multi-sheet workbook with:
  - Cover sheet with metadata
  - Consolidated 'All Categories' sheet with statistics
  - 10 category-specific sheets (Project Info, Business, Document, Technical,
    AI-ML, Organizational, Workflow, Risk, Future State, Vendor Selection)
  - Blue headers, alternating row colors, yellow customer response highlights
  - Working formulas linking consolidated sheet to category sheets
</commit_message>
<xml_diff>
--- a/solutions/aws/ai/intelligent-document-processing/presales/discovery-questionnaire.xlsx
+++ b/solutions/aws/ai/intelligent-document-processing/presales/discovery-questionnaire.xlsx
@@ -30,7 +30,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -88,17 +88,27 @@
       <sz val="12"/>
     </font>
     <font>
-      <name val="Segoe UI Semibold"/>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
       <b val="1"/>
       <sz val="11"/>
     </font>
-    <font>
-      <name val="Segoe UI Semibold"/>
-      <b val="1"/>
-      <sz val="12"/>
-    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill/>
     </fill>
@@ -131,6 +141,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="002F5496"/>
+        <bgColor rgb="002F5496"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F2F2F2"/>
+        <bgColor rgb="00F2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00FFF2CC"/>
         <bgColor rgb="00FFF2CC"/>
       </patternFill>
@@ -154,7 +176,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -190,11 +212,17 @@
         <color rgb="00DEE2E6"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -246,26 +274,29 @@
     <xf numFmtId="164" fontId="9" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="11" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="11" fillId="9" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -714,7 +745,7 @@
       </c>
       <c r="C7" s="6" t="inlineStr">
         <is>
-          <t>November 18, 2025</t>
+          <t>November 19, 2025</t>
         </is>
       </c>
     </row>
@@ -804,7 +835,7 @@
     <col width="30" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="32" customHeight="1">
+    <row r="1" ht="30" customHeight="1">
       <c r="A1" s="22" t="inlineStr">
         <is>
           <t>Question ID</t>
@@ -842,29 +873,29 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="inlineStr">
+      <c r="A2" s="25" t="inlineStr">
         <is>
           <t>RISK-001</t>
         </is>
       </c>
-      <c r="B2" s="10" t="inlineStr">
+      <c r="B2" s="25" t="inlineStr">
         <is>
           <t>Risk Assessment</t>
         </is>
       </c>
-      <c r="C2" s="10" t="inlineStr">
+      <c r="C2" s="25" t="inlineStr">
         <is>
           <t>Implementation</t>
         </is>
       </c>
-      <c r="D2" s="10" t="inlineStr">
+      <c r="D2" s="25" t="inlineStr">
         <is>
           <t>What are your main concerns about implementing IDP?</t>
         </is>
       </c>
-      <c r="E2" s="10" t="n"/>
-      <c r="F2" s="25" t="n"/>
-      <c r="G2" s="10" t="inlineStr">
+      <c r="E2" s="25" t="n"/>
+      <c r="F2" s="26" t="n"/>
+      <c r="G2" s="25" t="inlineStr">
         <is>
           <t>Primary implementation concerns</t>
         </is>
@@ -892,7 +923,7 @@
         </is>
       </c>
       <c r="E3" s="23" t="n"/>
-      <c r="F3" s="25" t="n"/>
+      <c r="F3" s="26" t="n"/>
       <c r="G3" s="23" t="inlineStr">
         <is>
           <t>Failure mode analysis</t>
@@ -900,29 +931,29 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="inlineStr">
+      <c r="A4" s="25" t="inlineStr">
         <is>
           <t>RISK-003</t>
         </is>
       </c>
-      <c r="B4" s="10" t="inlineStr">
+      <c r="B4" s="25" t="inlineStr">
         <is>
           <t>Risk Assessment</t>
         </is>
       </c>
-      <c r="C4" s="10" t="inlineStr">
+      <c r="C4" s="25" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
       </c>
-      <c r="D4" s="10" t="inlineStr">
+      <c r="D4" s="25" t="inlineStr">
         <is>
           <t>What are your concerns about data accuracy and quality?</t>
         </is>
       </c>
-      <c r="E4" s="10" t="n"/>
-      <c r="F4" s="25" t="n"/>
-      <c r="G4" s="10" t="inlineStr">
+      <c r="E4" s="25" t="n"/>
+      <c r="F4" s="26" t="n"/>
+      <c r="G4" s="25" t="inlineStr">
         <is>
           <t>Data quality risks</t>
         </is>
@@ -950,7 +981,7 @@
         </is>
       </c>
       <c r="E5" s="23" t="n"/>
-      <c r="F5" s="25" t="n"/>
+      <c r="F5" s="26" t="n"/>
       <c r="G5" s="23" t="inlineStr">
         <is>
           <t>Technical risk factors</t>
@@ -986,7 +1017,7 @@
     <col width="30" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="32" customHeight="1">
+    <row r="1" ht="30" customHeight="1">
       <c r="A1" s="22" t="inlineStr">
         <is>
           <t>Question ID</t>
@@ -1024,29 +1055,29 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="inlineStr">
+      <c r="A2" s="25" t="inlineStr">
         <is>
           <t>FUTURE-001</t>
         </is>
       </c>
-      <c r="B2" s="10" t="inlineStr">
+      <c r="B2" s="25" t="inlineStr">
         <is>
           <t>Future State</t>
         </is>
       </c>
-      <c r="C2" s="10" t="inlineStr">
+      <c r="C2" s="25" t="inlineStr">
         <is>
           <t>Vision</t>
         </is>
       </c>
-      <c r="D2" s="10" t="inlineStr">
+      <c r="D2" s="25" t="inlineStr">
         <is>
           <t>What is your long-term vision for document processing automation?</t>
         </is>
       </c>
-      <c r="E2" s="10" t="n"/>
-      <c r="F2" s="25" t="n"/>
-      <c r="G2" s="10" t="inlineStr">
+      <c r="E2" s="25" t="n"/>
+      <c r="F2" s="26" t="n"/>
+      <c r="G2" s="25" t="inlineStr">
         <is>
           <t>Future roadmap</t>
         </is>
@@ -1074,7 +1105,7 @@
         </is>
       </c>
       <c r="E3" s="23" t="n"/>
-      <c r="F3" s="25" t="n"/>
+      <c r="F3" s="26" t="n"/>
       <c r="G3" s="23" t="inlineStr">
         <is>
           <t>Scalability planning</t>
@@ -1082,29 +1113,29 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="inlineStr">
+      <c r="A4" s="25" t="inlineStr">
         <is>
           <t>FUTURE-003</t>
         </is>
       </c>
-      <c r="B4" s="10" t="inlineStr">
+      <c r="B4" s="25" t="inlineStr">
         <is>
           <t>Future State</t>
         </is>
       </c>
-      <c r="C4" s="10" t="inlineStr">
+      <c r="C4" s="25" t="inlineStr">
         <is>
           <t>Integration</t>
         </is>
       </c>
-      <c r="D4" s="10" t="inlineStr">
+      <c r="D4" s="25" t="inlineStr">
         <is>
           <t>What future document types or sources might need processing?</t>
         </is>
       </c>
-      <c r="E4" s="10" t="n"/>
-      <c r="F4" s="25" t="n"/>
-      <c r="G4" s="10" t="inlineStr">
+      <c r="E4" s="25" t="n"/>
+      <c r="F4" s="26" t="n"/>
+      <c r="G4" s="25" t="inlineStr">
         <is>
           <t>Future expansion needs</t>
         </is>
@@ -1139,7 +1170,7 @@
     <col width="30" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="32" customHeight="1">
+    <row r="1" ht="30" customHeight="1">
       <c r="A1" s="22" t="inlineStr">
         <is>
           <t>Question ID</t>
@@ -1177,29 +1208,29 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="inlineStr">
+      <c r="A2" s="25" t="inlineStr">
         <is>
           <t>ORG-007</t>
         </is>
       </c>
-      <c r="B2" s="10" t="inlineStr">
+      <c r="B2" s="25" t="inlineStr">
         <is>
           <t>Vendor Selection</t>
         </is>
       </c>
-      <c r="C2" s="10" t="inlineStr">
+      <c r="C2" s="25" t="inlineStr">
         <is>
           <t>Experience</t>
         </is>
       </c>
-      <c r="D2" s="10" t="inlineStr">
+      <c r="D2" s="25" t="inlineStr">
         <is>
           <t>What AWS AI/ML implementation experience do you expect from partners?</t>
         </is>
       </c>
-      <c r="E2" s="10" t="n"/>
-      <c r="F2" s="25" t="n"/>
-      <c r="G2" s="10" t="inlineStr">
+      <c r="E2" s="25" t="n"/>
+      <c r="F2" s="26" t="n"/>
+      <c r="G2" s="25" t="inlineStr">
         <is>
           <t>Partner requirements</t>
         </is>
@@ -1227,7 +1258,7 @@
         </is>
       </c>
       <c r="E3" s="23" t="n"/>
-      <c r="F3" s="25" t="n"/>
+      <c r="F3" s="26" t="n"/>
       <c r="G3" s="23" t="inlineStr">
         <is>
           <t>Support expectations</t>
@@ -1302,7 +1333,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" ht="32" customHeight="1">
+    <row r="4" ht="30" customHeight="1">
       <c r="A4" s="22" t="inlineStr">
         <is>
           <t>Question ID</t>
@@ -1370,23 +1401,23 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="10">
+      <c r="A6" s="25">
         <f>IF('Project Information'!A3="","",'Project Information'!A3)</f>
         <v/>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="25">
         <f>IF('Project Information'!B3="","",'Project Information'!B3)</f>
         <v/>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="25">
         <f>IF('Project Information'!C3="","",'Project Information'!C3)</f>
         <v/>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="25">
         <f>IF('Project Information'!D3="","",'Project Information'!D3)</f>
         <v/>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="25">
         <f>IF('Project Information'!E3="","",'Project Information'!E3)</f>
         <v/>
       </c>
@@ -1394,7 +1425,7 @@
         <f>IF('Project Information'!F3="","",'Project Information'!F3)</f>
         <v/>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="25">
         <f>IF('Project Information'!G3="","",'Project Information'!G3)</f>
         <v/>
       </c>
@@ -1430,23 +1461,23 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="10">
+      <c r="A8" s="25">
         <f>IF('Project Information'!A5="","",'Project Information'!A5)</f>
         <v/>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="25">
         <f>IF('Project Information'!B5="","",'Project Information'!B5)</f>
         <v/>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="25">
         <f>IF('Project Information'!C5="","",'Project Information'!C5)</f>
         <v/>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="25">
         <f>IF('Project Information'!D5="","",'Project Information'!D5)</f>
         <v/>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="25">
         <f>IF('Project Information'!E5="","",'Project Information'!E5)</f>
         <v/>
       </c>
@@ -1454,7 +1485,7 @@
         <f>IF('Project Information'!F5="","",'Project Information'!F5)</f>
         <v/>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="25">
         <f>IF('Project Information'!G5="","",'Project Information'!G5)</f>
         <v/>
       </c>
@@ -1490,23 +1521,23 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="10">
+      <c r="A10" s="25">
         <f>IF('Business Requirements'!A2="","",'Business Requirements'!A2)</f>
         <v/>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="25">
         <f>IF('Business Requirements'!B2="","",'Business Requirements'!B2)</f>
         <v/>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="25">
         <f>IF('Business Requirements'!C2="","",'Business Requirements'!C2)</f>
         <v/>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="25">
         <f>IF('Business Requirements'!D2="","",'Business Requirements'!D2)</f>
         <v/>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="25">
         <f>IF('Business Requirements'!E2="","",'Business Requirements'!E2)</f>
         <v/>
       </c>
@@ -1514,7 +1545,7 @@
         <f>IF('Business Requirements'!F2="","",'Business Requirements'!F2)</f>
         <v/>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="25">
         <f>IF('Business Requirements'!G2="","",'Business Requirements'!G2)</f>
         <v/>
       </c>
@@ -1550,23 +1581,23 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="10">
+      <c r="A12" s="25">
         <f>IF('Business Requirements'!A4="","",'Business Requirements'!A4)</f>
         <v/>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="25">
         <f>IF('Business Requirements'!B4="","",'Business Requirements'!B4)</f>
         <v/>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="25">
         <f>IF('Business Requirements'!C4="","",'Business Requirements'!C4)</f>
         <v/>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="25">
         <f>IF('Business Requirements'!D4="","",'Business Requirements'!D4)</f>
         <v/>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="25">
         <f>IF('Business Requirements'!E4="","",'Business Requirements'!E4)</f>
         <v/>
       </c>
@@ -1574,7 +1605,7 @@
         <f>IF('Business Requirements'!F4="","",'Business Requirements'!F4)</f>
         <v/>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="25">
         <f>IF('Business Requirements'!G4="","",'Business Requirements'!G4)</f>
         <v/>
       </c>
@@ -1610,23 +1641,23 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="10">
+      <c r="A14" s="25">
         <f>IF('Business Requirements'!A6="","",'Business Requirements'!A6)</f>
         <v/>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="25">
         <f>IF('Business Requirements'!B6="","",'Business Requirements'!B6)</f>
         <v/>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="25">
         <f>IF('Business Requirements'!C6="","",'Business Requirements'!C6)</f>
         <v/>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="25">
         <f>IF('Business Requirements'!D6="","",'Business Requirements'!D6)</f>
         <v/>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="25">
         <f>IF('Business Requirements'!E6="","",'Business Requirements'!E6)</f>
         <v/>
       </c>
@@ -1634,7 +1665,7 @@
         <f>IF('Business Requirements'!F6="","",'Business Requirements'!F6)</f>
         <v/>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="25">
         <f>IF('Business Requirements'!G6="","",'Business Requirements'!G6)</f>
         <v/>
       </c>
@@ -1670,23 +1701,23 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="10">
+      <c r="A16" s="25">
         <f>IF('Business Requirements'!A8="","",'Business Requirements'!A8)</f>
         <v/>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="25">
         <f>IF('Business Requirements'!B8="","",'Business Requirements'!B8)</f>
         <v/>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="25">
         <f>IF('Business Requirements'!C8="","",'Business Requirements'!C8)</f>
         <v/>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="25">
         <f>IF('Business Requirements'!D8="","",'Business Requirements'!D8)</f>
         <v/>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="25">
         <f>IF('Business Requirements'!E8="","",'Business Requirements'!E8)</f>
         <v/>
       </c>
@@ -1694,7 +1725,7 @@
         <f>IF('Business Requirements'!F8="","",'Business Requirements'!F8)</f>
         <v/>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="25">
         <f>IF('Business Requirements'!G8="","",'Business Requirements'!G8)</f>
         <v/>
       </c>
@@ -1730,23 +1761,23 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="10">
+      <c r="A18" s="25">
         <f>IF('Business Requirements'!A10="","",'Business Requirements'!A10)</f>
         <v/>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="25">
         <f>IF('Business Requirements'!B10="","",'Business Requirements'!B10)</f>
         <v/>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="25">
         <f>IF('Business Requirements'!C10="","",'Business Requirements'!C10)</f>
         <v/>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="25">
         <f>IF('Business Requirements'!D10="","",'Business Requirements'!D10)</f>
         <v/>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="25">
         <f>IF('Business Requirements'!E10="","",'Business Requirements'!E10)</f>
         <v/>
       </c>
@@ -1754,7 +1785,7 @@
         <f>IF('Business Requirements'!F10="","",'Business Requirements'!F10)</f>
         <v/>
       </c>
-      <c r="G18" s="10">
+      <c r="G18" s="25">
         <f>IF('Business Requirements'!G10="","",'Business Requirements'!G10)</f>
         <v/>
       </c>
@@ -1790,23 +1821,23 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="10">
+      <c r="A20" s="25">
         <f>IF('Document Requirements'!A2="","",'Document Requirements'!A2)</f>
         <v/>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="25">
         <f>IF('Document Requirements'!B2="","",'Document Requirements'!B2)</f>
         <v/>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="25">
         <f>IF('Document Requirements'!C2="","",'Document Requirements'!C2)</f>
         <v/>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="25">
         <f>IF('Document Requirements'!D2="","",'Document Requirements'!D2)</f>
         <v/>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="25">
         <f>IF('Document Requirements'!E2="","",'Document Requirements'!E2)</f>
         <v/>
       </c>
@@ -1814,7 +1845,7 @@
         <f>IF('Document Requirements'!F2="","",'Document Requirements'!F2)</f>
         <v/>
       </c>
-      <c r="G20" s="10">
+      <c r="G20" s="25">
         <f>IF('Document Requirements'!G2="","",'Document Requirements'!G2)</f>
         <v/>
       </c>
@@ -1850,23 +1881,23 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="10">
+      <c r="A22" s="25">
         <f>IF('Document Requirements'!A4="","",'Document Requirements'!A4)</f>
         <v/>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="25">
         <f>IF('Document Requirements'!B4="","",'Document Requirements'!B4)</f>
         <v/>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="25">
         <f>IF('Document Requirements'!C4="","",'Document Requirements'!C4)</f>
         <v/>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="25">
         <f>IF('Document Requirements'!D4="","",'Document Requirements'!D4)</f>
         <v/>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="25">
         <f>IF('Document Requirements'!E4="","",'Document Requirements'!E4)</f>
         <v/>
       </c>
@@ -1874,7 +1905,7 @@
         <f>IF('Document Requirements'!F4="","",'Document Requirements'!F4)</f>
         <v/>
       </c>
-      <c r="G22" s="10">
+      <c r="G22" s="25">
         <f>IF('Document Requirements'!G4="","",'Document Requirements'!G4)</f>
         <v/>
       </c>
@@ -1910,23 +1941,23 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="10">
+      <c r="A24" s="25">
         <f>IF('Document Requirements'!A6="","",'Document Requirements'!A6)</f>
         <v/>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="25">
         <f>IF('Document Requirements'!B6="","",'Document Requirements'!B6)</f>
         <v/>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="25">
         <f>IF('Document Requirements'!C6="","",'Document Requirements'!C6)</f>
         <v/>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="25">
         <f>IF('Document Requirements'!D6="","",'Document Requirements'!D6)</f>
         <v/>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="25">
         <f>IF('Document Requirements'!E6="","",'Document Requirements'!E6)</f>
         <v/>
       </c>
@@ -1934,7 +1965,7 @@
         <f>IF('Document Requirements'!F6="","",'Document Requirements'!F6)</f>
         <v/>
       </c>
-      <c r="G24" s="10">
+      <c r="G24" s="25">
         <f>IF('Document Requirements'!G6="","",'Document Requirements'!G6)</f>
         <v/>
       </c>
@@ -1970,23 +2001,23 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="10">
+      <c r="A26" s="25">
         <f>IF('Technical Requirements'!A2="","",'Technical Requirements'!A2)</f>
         <v/>
       </c>
-      <c r="B26" s="10">
+      <c r="B26" s="25">
         <f>IF('Technical Requirements'!B2="","",'Technical Requirements'!B2)</f>
         <v/>
       </c>
-      <c r="C26" s="10">
+      <c r="C26" s="25">
         <f>IF('Technical Requirements'!C2="","",'Technical Requirements'!C2)</f>
         <v/>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="25">
         <f>IF('Technical Requirements'!D2="","",'Technical Requirements'!D2)</f>
         <v/>
       </c>
-      <c r="E26" s="10">
+      <c r="E26" s="25">
         <f>IF('Technical Requirements'!E2="","",'Technical Requirements'!E2)</f>
         <v/>
       </c>
@@ -1994,7 +2025,7 @@
         <f>IF('Technical Requirements'!F2="","",'Technical Requirements'!F2)</f>
         <v/>
       </c>
-      <c r="G26" s="10">
+      <c r="G26" s="25">
         <f>IF('Technical Requirements'!G2="","",'Technical Requirements'!G2)</f>
         <v/>
       </c>
@@ -2030,23 +2061,23 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="10">
+      <c r="A28" s="25">
         <f>IF('Technical Requirements'!A4="","",'Technical Requirements'!A4)</f>
         <v/>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="25">
         <f>IF('Technical Requirements'!B4="","",'Technical Requirements'!B4)</f>
         <v/>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="25">
         <f>IF('Technical Requirements'!C4="","",'Technical Requirements'!C4)</f>
         <v/>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="25">
         <f>IF('Technical Requirements'!D4="","",'Technical Requirements'!D4)</f>
         <v/>
       </c>
-      <c r="E28" s="10">
+      <c r="E28" s="25">
         <f>IF('Technical Requirements'!E4="","",'Technical Requirements'!E4)</f>
         <v/>
       </c>
@@ -2054,7 +2085,7 @@
         <f>IF('Technical Requirements'!F4="","",'Technical Requirements'!F4)</f>
         <v/>
       </c>
-      <c r="G28" s="10">
+      <c r="G28" s="25">
         <f>IF('Technical Requirements'!G4="","",'Technical Requirements'!G4)</f>
         <v/>
       </c>
@@ -2090,23 +2121,23 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="10">
+      <c r="A30" s="25">
         <f>IF('Technical Requirements'!A6="","",'Technical Requirements'!A6)</f>
         <v/>
       </c>
-      <c r="B30" s="10">
+      <c r="B30" s="25">
         <f>IF('Technical Requirements'!B6="","",'Technical Requirements'!B6)</f>
         <v/>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="25">
         <f>IF('Technical Requirements'!C6="","",'Technical Requirements'!C6)</f>
         <v/>
       </c>
-      <c r="D30" s="10">
+      <c r="D30" s="25">
         <f>IF('Technical Requirements'!D6="","",'Technical Requirements'!D6)</f>
         <v/>
       </c>
-      <c r="E30" s="10">
+      <c r="E30" s="25">
         <f>IF('Technical Requirements'!E6="","",'Technical Requirements'!E6)</f>
         <v/>
       </c>
@@ -2114,7 +2145,7 @@
         <f>IF('Technical Requirements'!F6="","",'Technical Requirements'!F6)</f>
         <v/>
       </c>
-      <c r="G30" s="10">
+      <c r="G30" s="25">
         <f>IF('Technical Requirements'!G6="","",'Technical Requirements'!G6)</f>
         <v/>
       </c>
@@ -2150,23 +2181,23 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="10">
+      <c r="A32" s="25">
         <f>IF('Technical Requirements'!A8="","",'Technical Requirements'!A8)</f>
         <v/>
       </c>
-      <c r="B32" s="10">
+      <c r="B32" s="25">
         <f>IF('Technical Requirements'!B8="","",'Technical Requirements'!B8)</f>
         <v/>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="25">
         <f>IF('Technical Requirements'!C8="","",'Technical Requirements'!C8)</f>
         <v/>
       </c>
-      <c r="D32" s="10">
+      <c r="D32" s="25">
         <f>IF('Technical Requirements'!D8="","",'Technical Requirements'!D8)</f>
         <v/>
       </c>
-      <c r="E32" s="10">
+      <c r="E32" s="25">
         <f>IF('Technical Requirements'!E8="","",'Technical Requirements'!E8)</f>
         <v/>
       </c>
@@ -2174,7 +2205,7 @@
         <f>IF('Technical Requirements'!F8="","",'Technical Requirements'!F8)</f>
         <v/>
       </c>
-      <c r="G32" s="10">
+      <c r="G32" s="25">
         <f>IF('Technical Requirements'!G8="","",'Technical Requirements'!G8)</f>
         <v/>
       </c>
@@ -2210,23 +2241,23 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="10">
+      <c r="A34" s="25">
         <f>IF('Technical Requirements'!A10="","",'Technical Requirements'!A10)</f>
         <v/>
       </c>
-      <c r="B34" s="10">
+      <c r="B34" s="25">
         <f>IF('Technical Requirements'!B10="","",'Technical Requirements'!B10)</f>
         <v/>
       </c>
-      <c r="C34" s="10">
+      <c r="C34" s="25">
         <f>IF('Technical Requirements'!C10="","",'Technical Requirements'!C10)</f>
         <v/>
       </c>
-      <c r="D34" s="10">
+      <c r="D34" s="25">
         <f>IF('Technical Requirements'!D10="","",'Technical Requirements'!D10)</f>
         <v/>
       </c>
-      <c r="E34" s="10">
+      <c r="E34" s="25">
         <f>IF('Technical Requirements'!E10="","",'Technical Requirements'!E10)</f>
         <v/>
       </c>
@@ -2234,7 +2265,7 @@
         <f>IF('Technical Requirements'!F10="","",'Technical Requirements'!F10)</f>
         <v/>
       </c>
-      <c r="G34" s="10">
+      <c r="G34" s="25">
         <f>IF('Technical Requirements'!G10="","",'Technical Requirements'!G10)</f>
         <v/>
       </c>
@@ -2270,23 +2301,23 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="10">
+      <c r="A36" s="25">
         <f>IF('Technical Requirements'!A12="","",'Technical Requirements'!A12)</f>
         <v/>
       </c>
-      <c r="B36" s="10">
+      <c r="B36" s="25">
         <f>IF('Technical Requirements'!B12="","",'Technical Requirements'!B12)</f>
         <v/>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="25">
         <f>IF('Technical Requirements'!C12="","",'Technical Requirements'!C12)</f>
         <v/>
       </c>
-      <c r="D36" s="10">
+      <c r="D36" s="25">
         <f>IF('Technical Requirements'!D12="","",'Technical Requirements'!D12)</f>
         <v/>
       </c>
-      <c r="E36" s="10">
+      <c r="E36" s="25">
         <f>IF('Technical Requirements'!E12="","",'Technical Requirements'!E12)</f>
         <v/>
       </c>
@@ -2294,7 +2325,7 @@
         <f>IF('Technical Requirements'!F12="","",'Technical Requirements'!F12)</f>
         <v/>
       </c>
-      <c r="G36" s="10">
+      <c r="G36" s="25">
         <f>IF('Technical Requirements'!G12="","",'Technical Requirements'!G12)</f>
         <v/>
       </c>
@@ -2330,23 +2361,23 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="10">
+      <c r="A38" s="25">
         <f>IF('Technical Requirements'!A14="","",'Technical Requirements'!A14)</f>
         <v/>
       </c>
-      <c r="B38" s="10">
+      <c r="B38" s="25">
         <f>IF('Technical Requirements'!B14="","",'Technical Requirements'!B14)</f>
         <v/>
       </c>
-      <c r="C38" s="10">
+      <c r="C38" s="25">
         <f>IF('Technical Requirements'!C14="","",'Technical Requirements'!C14)</f>
         <v/>
       </c>
-      <c r="D38" s="10">
+      <c r="D38" s="25">
         <f>IF('Technical Requirements'!D14="","",'Technical Requirements'!D14)</f>
         <v/>
       </c>
-      <c r="E38" s="10">
+      <c r="E38" s="25">
         <f>IF('Technical Requirements'!E14="","",'Technical Requirements'!E14)</f>
         <v/>
       </c>
@@ -2354,7 +2385,7 @@
         <f>IF('Technical Requirements'!F14="","",'Technical Requirements'!F14)</f>
         <v/>
       </c>
-      <c r="G38" s="10">
+      <c r="G38" s="25">
         <f>IF('Technical Requirements'!G14="","",'Technical Requirements'!G14)</f>
         <v/>
       </c>
@@ -2390,23 +2421,23 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="10">
+      <c r="A40" s="25">
         <f>IF('AI-ML Requirements'!A3="","",'AI-ML Requirements'!A3)</f>
         <v/>
       </c>
-      <c r="B40" s="10">
+      <c r="B40" s="25">
         <f>IF('AI-ML Requirements'!B3="","",'AI-ML Requirements'!B3)</f>
         <v/>
       </c>
-      <c r="C40" s="10">
+      <c r="C40" s="25">
         <f>IF('AI-ML Requirements'!C3="","",'AI-ML Requirements'!C3)</f>
         <v/>
       </c>
-      <c r="D40" s="10">
+      <c r="D40" s="25">
         <f>IF('AI-ML Requirements'!D3="","",'AI-ML Requirements'!D3)</f>
         <v/>
       </c>
-      <c r="E40" s="10">
+      <c r="E40" s="25">
         <f>IF('AI-ML Requirements'!E3="","",'AI-ML Requirements'!E3)</f>
         <v/>
       </c>
@@ -2414,7 +2445,7 @@
         <f>IF('AI-ML Requirements'!F3="","",'AI-ML Requirements'!F3)</f>
         <v/>
       </c>
-      <c r="G40" s="10">
+      <c r="G40" s="25">
         <f>IF('AI-ML Requirements'!G3="","",'AI-ML Requirements'!G3)</f>
         <v/>
       </c>
@@ -2450,23 +2481,23 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="10">
+      <c r="A42" s="25">
         <f>IF('AI-ML Requirements'!A5="","",'AI-ML Requirements'!A5)</f>
         <v/>
       </c>
-      <c r="B42" s="10">
+      <c r="B42" s="25">
         <f>IF('AI-ML Requirements'!B5="","",'AI-ML Requirements'!B5)</f>
         <v/>
       </c>
-      <c r="C42" s="10">
+      <c r="C42" s="25">
         <f>IF('AI-ML Requirements'!C5="","",'AI-ML Requirements'!C5)</f>
         <v/>
       </c>
-      <c r="D42" s="10">
+      <c r="D42" s="25">
         <f>IF('AI-ML Requirements'!D5="","",'AI-ML Requirements'!D5)</f>
         <v/>
       </c>
-      <c r="E42" s="10">
+      <c r="E42" s="25">
         <f>IF('AI-ML Requirements'!E5="","",'AI-ML Requirements'!E5)</f>
         <v/>
       </c>
@@ -2474,7 +2505,7 @@
         <f>IF('AI-ML Requirements'!F5="","",'AI-ML Requirements'!F5)</f>
         <v/>
       </c>
-      <c r="G42" s="10">
+      <c r="G42" s="25">
         <f>IF('AI-ML Requirements'!G5="","",'AI-ML Requirements'!G5)</f>
         <v/>
       </c>
@@ -2510,23 +2541,23 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="10">
+      <c r="A44" s="25">
         <f>IF('Organizational'!A3="","",'Organizational'!A3)</f>
         <v/>
       </c>
-      <c r="B44" s="10">
+      <c r="B44" s="25">
         <f>IF('Organizational'!B3="","",'Organizational'!B3)</f>
         <v/>
       </c>
-      <c r="C44" s="10">
+      <c r="C44" s="25">
         <f>IF('Organizational'!C3="","",'Organizational'!C3)</f>
         <v/>
       </c>
-      <c r="D44" s="10">
+      <c r="D44" s="25">
         <f>IF('Organizational'!D3="","",'Organizational'!D3)</f>
         <v/>
       </c>
-      <c r="E44" s="10">
+      <c r="E44" s="25">
         <f>IF('Organizational'!E3="","",'Organizational'!E3)</f>
         <v/>
       </c>
@@ -2534,7 +2565,7 @@
         <f>IF('Organizational'!F3="","",'Organizational'!F3)</f>
         <v/>
       </c>
-      <c r="G44" s="10">
+      <c r="G44" s="25">
         <f>IF('Organizational'!G3="","",'Organizational'!G3)</f>
         <v/>
       </c>
@@ -2570,23 +2601,23 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="10">
+      <c r="A46" s="25">
         <f>IF('Organizational'!A5="","",'Organizational'!A5)</f>
         <v/>
       </c>
-      <c r="B46" s="10">
+      <c r="B46" s="25">
         <f>IF('Organizational'!B5="","",'Organizational'!B5)</f>
         <v/>
       </c>
-      <c r="C46" s="10">
+      <c r="C46" s="25">
         <f>IF('Organizational'!C5="","",'Organizational'!C5)</f>
         <v/>
       </c>
-      <c r="D46" s="10">
+      <c r="D46" s="25">
         <f>IF('Organizational'!D5="","",'Organizational'!D5)</f>
         <v/>
       </c>
-      <c r="E46" s="10">
+      <c r="E46" s="25">
         <f>IF('Organizational'!E5="","",'Organizational'!E5)</f>
         <v/>
       </c>
@@ -2594,7 +2625,7 @@
         <f>IF('Organizational'!F5="","",'Organizational'!F5)</f>
         <v/>
       </c>
-      <c r="G46" s="10">
+      <c r="G46" s="25">
         <f>IF('Organizational'!G5="","",'Organizational'!G5)</f>
         <v/>
       </c>
@@ -2630,23 +2661,23 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="10">
+      <c r="A48" s="25">
         <f>IF('Organizational'!A7="","",'Organizational'!A7)</f>
         <v/>
       </c>
-      <c r="B48" s="10">
+      <c r="B48" s="25">
         <f>IF('Organizational'!B7="","",'Organizational'!B7)</f>
         <v/>
       </c>
-      <c r="C48" s="10">
+      <c r="C48" s="25">
         <f>IF('Organizational'!C7="","",'Organizational'!C7)</f>
         <v/>
       </c>
-      <c r="D48" s="10">
+      <c r="D48" s="25">
         <f>IF('Organizational'!D7="","",'Organizational'!D7)</f>
         <v/>
       </c>
-      <c r="E48" s="10">
+      <c r="E48" s="25">
         <f>IF('Organizational'!E7="","",'Organizational'!E7)</f>
         <v/>
       </c>
@@ -2654,7 +2685,7 @@
         <f>IF('Organizational'!F7="","",'Organizational'!F7)</f>
         <v/>
       </c>
-      <c r="G48" s="10">
+      <c r="G48" s="25">
         <f>IF('Organizational'!G7="","",'Organizational'!G7)</f>
         <v/>
       </c>
@@ -2690,23 +2721,23 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="10">
+      <c r="A50" s="25">
         <f>IF('Workflow Requirements'!A3="","",'Workflow Requirements'!A3)</f>
         <v/>
       </c>
-      <c r="B50" s="10">
+      <c r="B50" s="25">
         <f>IF('Workflow Requirements'!B3="","",'Workflow Requirements'!B3)</f>
         <v/>
       </c>
-      <c r="C50" s="10">
+      <c r="C50" s="25">
         <f>IF('Workflow Requirements'!C3="","",'Workflow Requirements'!C3)</f>
         <v/>
       </c>
-      <c r="D50" s="10">
+      <c r="D50" s="25">
         <f>IF('Workflow Requirements'!D3="","",'Workflow Requirements'!D3)</f>
         <v/>
       </c>
-      <c r="E50" s="10">
+      <c r="E50" s="25">
         <f>IF('Workflow Requirements'!E3="","",'Workflow Requirements'!E3)</f>
         <v/>
       </c>
@@ -2714,7 +2745,7 @@
         <f>IF('Workflow Requirements'!F3="","",'Workflow Requirements'!F3)</f>
         <v/>
       </c>
-      <c r="G50" s="10">
+      <c r="G50" s="25">
         <f>IF('Workflow Requirements'!G3="","",'Workflow Requirements'!G3)</f>
         <v/>
       </c>
@@ -2750,23 +2781,23 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="10">
+      <c r="A52" s="25">
         <f>IF('Workflow Requirements'!A5="","",'Workflow Requirements'!A5)</f>
         <v/>
       </c>
-      <c r="B52" s="10">
+      <c r="B52" s="25">
         <f>IF('Workflow Requirements'!B5="","",'Workflow Requirements'!B5)</f>
         <v/>
       </c>
-      <c r="C52" s="10">
+      <c r="C52" s="25">
         <f>IF('Workflow Requirements'!C5="","",'Workflow Requirements'!C5)</f>
         <v/>
       </c>
-      <c r="D52" s="10">
+      <c r="D52" s="25">
         <f>IF('Workflow Requirements'!D5="","",'Workflow Requirements'!D5)</f>
         <v/>
       </c>
-      <c r="E52" s="10">
+      <c r="E52" s="25">
         <f>IF('Workflow Requirements'!E5="","",'Workflow Requirements'!E5)</f>
         <v/>
       </c>
@@ -2774,7 +2805,7 @@
         <f>IF('Workflow Requirements'!F5="","",'Workflow Requirements'!F5)</f>
         <v/>
       </c>
-      <c r="G52" s="10">
+      <c r="G52" s="25">
         <f>IF('Workflow Requirements'!G5="","",'Workflow Requirements'!G5)</f>
         <v/>
       </c>
@@ -2810,23 +2841,23 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="10">
+      <c r="A54" s="25">
         <f>IF('Risk Assessment'!A3="","",'Risk Assessment'!A3)</f>
         <v/>
       </c>
-      <c r="B54" s="10">
+      <c r="B54" s="25">
         <f>IF('Risk Assessment'!B3="","",'Risk Assessment'!B3)</f>
         <v/>
       </c>
-      <c r="C54" s="10">
+      <c r="C54" s="25">
         <f>IF('Risk Assessment'!C3="","",'Risk Assessment'!C3)</f>
         <v/>
       </c>
-      <c r="D54" s="10">
+      <c r="D54" s="25">
         <f>IF('Risk Assessment'!D3="","",'Risk Assessment'!D3)</f>
         <v/>
       </c>
-      <c r="E54" s="10">
+      <c r="E54" s="25">
         <f>IF('Risk Assessment'!E3="","",'Risk Assessment'!E3)</f>
         <v/>
       </c>
@@ -2834,7 +2865,7 @@
         <f>IF('Risk Assessment'!F3="","",'Risk Assessment'!F3)</f>
         <v/>
       </c>
-      <c r="G54" s="10">
+      <c r="G54" s="25">
         <f>IF('Risk Assessment'!G3="","",'Risk Assessment'!G3)</f>
         <v/>
       </c>
@@ -2870,23 +2901,23 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="10">
+      <c r="A56" s="25">
         <f>IF('Risk Assessment'!A5="","",'Risk Assessment'!A5)</f>
         <v/>
       </c>
-      <c r="B56" s="10">
+      <c r="B56" s="25">
         <f>IF('Risk Assessment'!B5="","",'Risk Assessment'!B5)</f>
         <v/>
       </c>
-      <c r="C56" s="10">
+      <c r="C56" s="25">
         <f>IF('Risk Assessment'!C5="","",'Risk Assessment'!C5)</f>
         <v/>
       </c>
-      <c r="D56" s="10">
+      <c r="D56" s="25">
         <f>IF('Risk Assessment'!D5="","",'Risk Assessment'!D5)</f>
         <v/>
       </c>
-      <c r="E56" s="10">
+      <c r="E56" s="25">
         <f>IF('Risk Assessment'!E5="","",'Risk Assessment'!E5)</f>
         <v/>
       </c>
@@ -2894,7 +2925,7 @@
         <f>IF('Risk Assessment'!F5="","",'Risk Assessment'!F5)</f>
         <v/>
       </c>
-      <c r="G56" s="10">
+      <c r="G56" s="25">
         <f>IF('Risk Assessment'!G5="","",'Risk Assessment'!G5)</f>
         <v/>
       </c>
@@ -2930,23 +2961,23 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="10">
+      <c r="A58" s="25">
         <f>IF('Future State'!A3="","",'Future State'!A3)</f>
         <v/>
       </c>
-      <c r="B58" s="10">
+      <c r="B58" s="25">
         <f>IF('Future State'!B3="","",'Future State'!B3)</f>
         <v/>
       </c>
-      <c r="C58" s="10">
+      <c r="C58" s="25">
         <f>IF('Future State'!C3="","",'Future State'!C3)</f>
         <v/>
       </c>
-      <c r="D58" s="10">
+      <c r="D58" s="25">
         <f>IF('Future State'!D3="","",'Future State'!D3)</f>
         <v/>
       </c>
-      <c r="E58" s="10">
+      <c r="E58" s="25">
         <f>IF('Future State'!E3="","",'Future State'!E3)</f>
         <v/>
       </c>
@@ -2954,7 +2985,7 @@
         <f>IF('Future State'!F3="","",'Future State'!F3)</f>
         <v/>
       </c>
-      <c r="G58" s="10">
+      <c r="G58" s="25">
         <f>IF('Future State'!G3="","",'Future State'!G3)</f>
         <v/>
       </c>
@@ -2990,23 +3021,23 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="10">
+      <c r="A60" s="25">
         <f>IF('Vendor Selection'!A2="","",'Vendor Selection'!A2)</f>
         <v/>
       </c>
-      <c r="B60" s="10">
+      <c r="B60" s="25">
         <f>IF('Vendor Selection'!B2="","",'Vendor Selection'!B2)</f>
         <v/>
       </c>
-      <c r="C60" s="10">
+      <c r="C60" s="25">
         <f>IF('Vendor Selection'!C2="","",'Vendor Selection'!C2)</f>
         <v/>
       </c>
-      <c r="D60" s="10">
+      <c r="D60" s="25">
         <f>IF('Vendor Selection'!D2="","",'Vendor Selection'!D2)</f>
         <v/>
       </c>
-      <c r="E60" s="10">
+      <c r="E60" s="25">
         <f>IF('Vendor Selection'!E2="","",'Vendor Selection'!E2)</f>
         <v/>
       </c>
@@ -3014,7 +3045,7 @@
         <f>IF('Vendor Selection'!F2="","",'Vendor Selection'!F2)</f>
         <v/>
       </c>
-      <c r="G60" s="10">
+      <c r="G60" s="25">
         <f>IF('Vendor Selection'!G2="","",'Vendor Selection'!G2)</f>
         <v/>
       </c>
@@ -3079,7 +3110,7 @@
     <col width="30" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="32" customHeight="1">
+    <row r="1" ht="30" customHeight="1">
       <c r="A1" s="22" t="inlineStr">
         <is>
           <t>Question ID</t>
@@ -3117,29 +3148,29 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="inlineStr">
+      <c r="A2" s="25" t="inlineStr">
         <is>
           <t>PROJ-001</t>
         </is>
       </c>
-      <c r="B2" s="10" t="inlineStr">
+      <c r="B2" s="25" t="inlineStr">
         <is>
           <t>Project Information</t>
         </is>
       </c>
-      <c r="C2" s="10" t="inlineStr">
+      <c r="C2" s="25" t="inlineStr">
         <is>
           <t>Basic Details</t>
         </is>
       </c>
-      <c r="D2" s="10" t="inlineStr">
+      <c r="D2" s="25" t="inlineStr">
         <is>
           <t>What is the name of your Intelligent Document Processing solution?</t>
         </is>
       </c>
-      <c r="E2" s="10" t="n"/>
-      <c r="F2" s="25" t="n"/>
-      <c r="G2" s="10" t="inlineStr">
+      <c r="E2" s="25" t="n"/>
+      <c r="F2" s="26" t="n"/>
+      <c r="G2" s="25" t="inlineStr">
         <is>
           <t>Internal project reference</t>
         </is>
@@ -3167,7 +3198,7 @@
         </is>
       </c>
       <c r="E3" s="23" t="n"/>
-      <c r="F3" s="25" t="n"/>
+      <c r="F3" s="26" t="n"/>
       <c r="G3" s="23" t="inlineStr">
         <is>
           <t>Client identification</t>
@@ -3175,29 +3206,29 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="inlineStr">
+      <c r="A4" s="25" t="inlineStr">
         <is>
           <t>PROJ-003</t>
         </is>
       </c>
-      <c r="B4" s="10" t="inlineStr">
+      <c r="B4" s="25" t="inlineStr">
         <is>
           <t>Project Information</t>
         </is>
       </c>
-      <c r="C4" s="10" t="inlineStr">
+      <c r="C4" s="25" t="inlineStr">
         <is>
           <t>Basic Details</t>
         </is>
       </c>
-      <c r="D4" s="10" t="inlineStr">
+      <c r="D4" s="25" t="inlineStr">
         <is>
           <t>Who is the primary stakeholder for this IDP project?</t>
         </is>
       </c>
-      <c r="E4" s="10" t="n"/>
-      <c r="F4" s="25" t="n"/>
-      <c r="G4" s="10" t="inlineStr">
+      <c r="E4" s="25" t="n"/>
+      <c r="F4" s="26" t="n"/>
+      <c r="G4" s="25" t="inlineStr">
         <is>
           <t>Main point of contact</t>
         </is>
@@ -3225,7 +3256,7 @@
         </is>
       </c>
       <c r="E5" s="23" t="n"/>
-      <c r="F5" s="25" t="n"/>
+      <c r="F5" s="26" t="n"/>
       <c r="G5" s="23" t="inlineStr">
         <is>
           <t>Decision-making authority</t>
@@ -3233,29 +3264,29 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="10" t="inlineStr">
+      <c r="A6" s="25" t="inlineStr">
         <is>
           <t>PROJ-005</t>
         </is>
       </c>
-      <c r="B6" s="10" t="inlineStr">
+      <c r="B6" s="25" t="inlineStr">
         <is>
           <t>Project Information</t>
         </is>
       </c>
-      <c r="C6" s="10" t="inlineStr">
+      <c r="C6" s="25" t="inlineStr">
         <is>
           <t>Basic Details</t>
         </is>
       </c>
-      <c r="D6" s="10" t="inlineStr">
+      <c r="D6" s="25" t="inlineStr">
         <is>
           <t>What is today's date?</t>
         </is>
       </c>
-      <c r="E6" s="10" t="n"/>
-      <c r="F6" s="25" t="n"/>
-      <c r="G6" s="10" t="inlineStr">
+      <c r="E6" s="25" t="n"/>
+      <c r="F6" s="26" t="n"/>
+      <c r="G6" s="25" t="inlineStr">
         <is>
           <t>Questionnaire completion date</t>
         </is>
@@ -3290,7 +3321,7 @@
     <col width="30" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="32" customHeight="1">
+    <row r="1" ht="30" customHeight="1">
       <c r="A1" s="22" t="inlineStr">
         <is>
           <t>Question ID</t>
@@ -3328,33 +3359,33 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="inlineStr">
+      <c r="A2" s="25" t="inlineStr">
         <is>
           <t>BUS-001</t>
         </is>
       </c>
-      <c r="B2" s="10" t="inlineStr">
+      <c r="B2" s="25" t="inlineStr">
         <is>
           <t>Business Requirements</t>
         </is>
       </c>
-      <c r="C2" s="10" t="inlineStr">
+      <c r="C2" s="25" t="inlineStr">
         <is>
           <t>Current State</t>
         </is>
       </c>
-      <c r="D2" s="10" t="inlineStr">
+      <c r="D2" s="25" t="inlineStr">
         <is>
           <t>What document processing challenges are you trying to solve?</t>
         </is>
       </c>
-      <c r="E2" s="10" t="inlineStr">
+      <c r="E2" s="25" t="inlineStr">
         <is>
           <t>Common challenges: Manual data entry, Document classification errors, Slow processing times, High operational costs, Compliance issues, Data accuracy problems</t>
         </is>
       </c>
-      <c r="F2" s="25" t="n"/>
-      <c r="G2" s="10" t="inlineStr">
+      <c r="F2" s="26" t="n"/>
+      <c r="G2" s="25" t="inlineStr">
         <is>
           <t>Primary business driver for IDP</t>
         </is>
@@ -3382,7 +3413,7 @@
         </is>
       </c>
       <c r="E3" s="23" t="n"/>
-      <c r="F3" s="25" t="n"/>
+      <c r="F3" s="26" t="n"/>
       <c r="G3" s="23" t="inlineStr">
         <is>
           <t>Current state assessment</t>
@@ -3390,33 +3421,33 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="inlineStr">
+      <c r="A4" s="25" t="inlineStr">
         <is>
           <t>BUS-003</t>
         </is>
       </c>
-      <c r="B4" s="10" t="inlineStr">
+      <c r="B4" s="25" t="inlineStr">
         <is>
           <t>Business Requirements</t>
         </is>
       </c>
-      <c r="C4" s="10" t="inlineStr">
+      <c r="C4" s="25" t="inlineStr">
         <is>
           <t>Current State</t>
         </is>
       </c>
-      <c r="D4" s="10" t="inlineStr">
+      <c r="D4" s="25" t="inlineStr">
         <is>
           <t>What types of documents do you process regularly?</t>
         </is>
       </c>
-      <c r="E4" s="10" t="inlineStr">
+      <c r="E4" s="25" t="inlineStr">
         <is>
           <t>Common types: Invoices, Contracts, Insurance claims, Medical records, Tax documents, Legal documents, Forms, Letters</t>
         </is>
       </c>
-      <c r="F4" s="25" t="n"/>
-      <c r="G4" s="10" t="inlineStr">
+      <c r="F4" s="26" t="n"/>
+      <c r="G4" s="25" t="inlineStr">
         <is>
           <t>Document type classification</t>
         </is>
@@ -3448,7 +3479,7 @@
           <t>Typical ranges: 1-100, 101-1000, 1001-10000, 10000+</t>
         </is>
       </c>
-      <c r="F5" s="25" t="n"/>
+      <c r="F5" s="26" t="n"/>
       <c r="G5" s="23" t="inlineStr">
         <is>
           <t>Processing volume requirements</t>
@@ -3456,33 +3487,33 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="10" t="inlineStr">
+      <c r="A6" s="25" t="inlineStr">
         <is>
           <t>BUS-005</t>
         </is>
       </c>
-      <c r="B6" s="10" t="inlineStr">
+      <c r="B6" s="25" t="inlineStr">
         <is>
           <t>Business Requirements</t>
         </is>
       </c>
-      <c r="C6" s="10" t="inlineStr">
+      <c r="C6" s="25" t="inlineStr">
         <is>
           <t>Current State</t>
         </is>
       </c>
-      <c r="D6" s="10" t="inlineStr">
+      <c r="D6" s="25" t="inlineStr">
         <is>
           <t>What document formats do you currently handle?</t>
         </is>
       </c>
-      <c r="E6" s="10" t="inlineStr">
+      <c r="E6" s="25" t="inlineStr">
         <is>
           <t>Common formats: PDF, Word documents, Scanned images, Handwritten documents, Multi-page documents, Email attachments, Fax documents</t>
         </is>
       </c>
-      <c r="F6" s="25" t="n"/>
-      <c r="G6" s="10" t="inlineStr">
+      <c r="F6" s="26" t="n"/>
+      <c r="G6" s="25" t="inlineStr">
         <is>
           <t>Input format requirements</t>
         </is>
@@ -3514,7 +3545,7 @@
           <t>Common goals: Reduce manual data entry, Improve processing speed, Increase accuracy, Lower operational costs, Ensure compliance, Enable scalability</t>
         </is>
       </c>
-      <c r="F7" s="25" t="n"/>
+      <c r="F7" s="26" t="n"/>
       <c r="G7" s="23" t="inlineStr">
         <is>
           <t>Business objectives</t>
@@ -3522,29 +3553,29 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="10" t="inlineStr">
+      <c r="A8" s="25" t="inlineStr">
         <is>
           <t>BUS-007</t>
         </is>
       </c>
-      <c r="B8" s="10" t="inlineStr">
+      <c r="B8" s="25" t="inlineStr">
         <is>
           <t>Business Requirements</t>
         </is>
       </c>
-      <c r="C8" s="10" t="inlineStr">
+      <c r="C8" s="25" t="inlineStr">
         <is>
           <t>Objectives</t>
         </is>
       </c>
-      <c r="D8" s="10" t="inlineStr">
+      <c r="D8" s="25" t="inlineStr">
         <is>
           <t>What specific data do you need to extract from documents?</t>
         </is>
       </c>
-      <c r="E8" s="10" t="n"/>
-      <c r="F8" s="25" t="n"/>
-      <c r="G8" s="10" t="inlineStr">
+      <c r="E8" s="25" t="n"/>
+      <c r="F8" s="26" t="n"/>
+      <c r="G8" s="25" t="inlineStr">
         <is>
           <t>Data extraction requirements</t>
         </is>
@@ -3576,7 +3607,7 @@
           <t>Typical ranges: 0-3 months, 3-6 months, 6-12 months, 12+ months</t>
         </is>
       </c>
-      <c r="F9" s="25" t="n"/>
+      <c r="F9" s="26" t="n"/>
       <c r="G9" s="23" t="inlineStr">
         <is>
           <t>Project timeline expectations</t>
@@ -3584,33 +3615,33 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="inlineStr">
+      <c r="A10" s="25" t="inlineStr">
         <is>
           <t>BUS-009</t>
         </is>
       </c>
-      <c r="B10" s="10" t="inlineStr">
+      <c r="B10" s="25" t="inlineStr">
         <is>
           <t>Business Requirements</t>
         </is>
       </c>
-      <c r="C10" s="10" t="inlineStr">
+      <c r="C10" s="25" t="inlineStr">
         <is>
           <t>Budget</t>
         </is>
       </c>
-      <c r="D10" s="10" t="inlineStr">
+      <c r="D10" s="25" t="inlineStr">
         <is>
           <t>What is your approved budget range for this IDP solution?</t>
         </is>
       </c>
-      <c r="E10" s="10" t="inlineStr">
+      <c r="E10" s="25" t="inlineStr">
         <is>
           <t>Common ranges: $0-50K, $50K-250K, $250K-1M, $1M+</t>
         </is>
       </c>
-      <c r="F10" s="25" t="n"/>
-      <c r="G10" s="10" t="inlineStr">
+      <c r="F10" s="26" t="n"/>
+      <c r="G10" s="25" t="inlineStr">
         <is>
           <t>Budget constraints</t>
         </is>
@@ -3638,7 +3669,7 @@
         </is>
       </c>
       <c r="E11" s="23" t="n"/>
-      <c r="F11" s="25" t="n"/>
+      <c r="F11" s="26" t="n"/>
       <c r="G11" s="23" t="inlineStr">
         <is>
           <t>KPI definition for document processing</t>
@@ -3674,7 +3705,7 @@
     <col width="30" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="32" customHeight="1">
+    <row r="1" ht="30" customHeight="1">
       <c r="A1" s="22" t="inlineStr">
         <is>
           <t>Question ID</t>
@@ -3712,29 +3743,29 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="inlineStr">
+      <c r="A2" s="25" t="inlineStr">
         <is>
           <t>DOC-001</t>
         </is>
       </c>
-      <c r="B2" s="10" t="inlineStr">
+      <c r="B2" s="25" t="inlineStr">
         <is>
           <t>Document Requirements</t>
         </is>
       </c>
-      <c r="C2" s="10" t="inlineStr">
+      <c r="C2" s="25" t="inlineStr">
         <is>
           <t>Types</t>
         </is>
       </c>
-      <c r="D2" s="10" t="inlineStr">
+      <c r="D2" s="25" t="inlineStr">
         <is>
           <t>What specific document types need automated processing?</t>
         </is>
       </c>
-      <c r="E2" s="10" t="n"/>
-      <c r="F2" s="25" t="n"/>
-      <c r="G2" s="10" t="inlineStr">
+      <c r="E2" s="25" t="n"/>
+      <c r="F2" s="26" t="n"/>
+      <c r="G2" s="25" t="inlineStr">
         <is>
           <t>Detailed document classification</t>
         </is>
@@ -3766,7 +3797,7 @@
           <t>Types: Structured forms, Semi-structured invoices, Unstructured letters, Mixed types</t>
         </is>
       </c>
-      <c r="F3" s="25" t="n"/>
+      <c r="F3" s="26" t="n"/>
       <c r="G3" s="23" t="inlineStr">
         <is>
           <t>Document structure analysis</t>
@@ -3774,33 +3805,33 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="inlineStr">
+      <c r="A4" s="25" t="inlineStr">
         <is>
           <t>DOC-003</t>
         </is>
       </c>
-      <c r="B4" s="10" t="inlineStr">
+      <c r="B4" s="25" t="inlineStr">
         <is>
           <t>Document Requirements</t>
         </is>
       </c>
-      <c r="C4" s="10" t="inlineStr">
+      <c r="C4" s="25" t="inlineStr">
         <is>
           <t>Quality</t>
         </is>
       </c>
-      <c r="D4" s="10" t="inlineStr">
+      <c r="D4" s="25" t="inlineStr">
         <is>
           <t>What is the typical quality of your source documents?</t>
         </is>
       </c>
-      <c r="E4" s="10" t="inlineStr">
+      <c r="E4" s="25" t="inlineStr">
         <is>
           <t>Quality levels: High quality digital, Good quality scanned, Poor quality scanned, Handwritten, Mixed quality</t>
         </is>
       </c>
-      <c r="F4" s="25" t="n"/>
-      <c r="G4" s="10" t="inlineStr">
+      <c r="F4" s="26" t="n"/>
+      <c r="G4" s="25" t="inlineStr">
         <is>
           <t>OCR accuracy expectations</t>
         </is>
@@ -3828,7 +3859,7 @@
         </is>
       </c>
       <c r="E5" s="23" t="n"/>
-      <c r="F5" s="25" t="n"/>
+      <c r="F5" s="26" t="n"/>
       <c r="G5" s="23" t="inlineStr">
         <is>
           <t>Multi-language processing needs</t>
@@ -3836,33 +3867,33 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="10" t="inlineStr">
+      <c r="A6" s="25" t="inlineStr">
         <is>
           <t>DOC-005</t>
         </is>
       </c>
-      <c r="B6" s="10" t="inlineStr">
+      <c r="B6" s="25" t="inlineStr">
         <is>
           <t>Document Requirements</t>
         </is>
       </c>
-      <c r="C6" s="10" t="inlineStr">
+      <c r="C6" s="25" t="inlineStr">
         <is>
           <t>Variations</t>
         </is>
       </c>
-      <c r="D6" s="10" t="inlineStr">
+      <c r="D6" s="25" t="inlineStr">
         <is>
           <t>How much variation exists within each document type?</t>
         </is>
       </c>
-      <c r="E6" s="10" t="inlineStr">
+      <c r="E6" s="25" t="inlineStr">
         <is>
           <t>Variation levels: Highly standardized, Some variation, Significant variation, Completely variable</t>
         </is>
       </c>
-      <c r="F6" s="25" t="n"/>
-      <c r="G6" s="10" t="inlineStr">
+      <c r="F6" s="26" t="n"/>
+      <c r="G6" s="25" t="inlineStr">
         <is>
           <t>Model training complexity</t>
         </is>
@@ -3890,7 +3921,7 @@
         </is>
       </c>
       <c r="E7" s="23" t="n"/>
-      <c r="F7" s="25" t="n"/>
+      <c r="F7" s="26" t="n"/>
       <c r="G7" s="23" t="inlineStr">
         <is>
           <t>Input channel requirements</t>
@@ -3926,7 +3957,7 @@
     <col width="30" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="32" customHeight="1">
+    <row r="1" ht="30" customHeight="1">
       <c r="A1" s="22" t="inlineStr">
         <is>
           <t>Question ID</t>
@@ -3964,33 +3995,33 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="inlineStr">
+      <c r="A2" s="25" t="inlineStr">
         <is>
           <t>TECH-001</t>
         </is>
       </c>
-      <c r="B2" s="10" t="inlineStr">
+      <c r="B2" s="25" t="inlineStr">
         <is>
           <t>Technical Requirements</t>
         </is>
       </c>
-      <c r="C2" s="10" t="inlineStr">
+      <c r="C2" s="25" t="inlineStr">
         <is>
           <t>AWS Environment</t>
         </is>
       </c>
-      <c r="D2" s="10" t="inlineStr">
+      <c r="D2" s="25" t="inlineStr">
         <is>
           <t>What AWS services are you currently using?</t>
         </is>
       </c>
-      <c r="E2" s="10" t="inlineStr">
+      <c r="E2" s="25" t="inlineStr">
         <is>
           <t>AWS services: S3, Lambda, API Gateway, Textract, Comprehend, SageMaker, None, Other</t>
         </is>
       </c>
-      <c r="F2" s="25" t="n"/>
-      <c r="G2" s="10" t="inlineStr">
+      <c r="F2" s="26" t="n"/>
+      <c r="G2" s="25" t="inlineStr">
         <is>
           <t>Current AWS footprint</t>
         </is>
@@ -4018,7 +4049,7 @@
         </is>
       </c>
       <c r="E3" s="23" t="n"/>
-      <c r="F3" s="25" t="n"/>
+      <c r="F3" s="26" t="n"/>
       <c r="G3" s="23" t="inlineStr">
         <is>
           <t>Data residency requirements</t>
@@ -4026,29 +4057,29 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="inlineStr">
+      <c r="A4" s="25" t="inlineStr">
         <is>
           <t>TECH-003</t>
         </is>
       </c>
-      <c r="B4" s="10" t="inlineStr">
+      <c r="B4" s="25" t="inlineStr">
         <is>
           <t>Technical Requirements</t>
         </is>
       </c>
-      <c r="C4" s="10" t="inlineStr">
+      <c r="C4" s="25" t="inlineStr">
         <is>
           <t>Integration</t>
         </is>
       </c>
-      <c r="D4" s="10" t="inlineStr">
+      <c r="D4" s="25" t="inlineStr">
         <is>
           <t>What systems need to integrate with the IDP solution?</t>
         </is>
       </c>
-      <c r="E4" s="10" t="n"/>
-      <c r="F4" s="25" t="n"/>
-      <c r="G4" s="10" t="inlineStr">
+      <c r="E4" s="25" t="n"/>
+      <c r="F4" s="26" t="n"/>
+      <c r="G4" s="25" t="inlineStr">
         <is>
           <t>Integration requirements</t>
         </is>
@@ -4080,7 +4111,7 @@
           <t>Common systems: AWS S3, SharePoint, Google Drive, Box, On-premises file servers, Email systems</t>
         </is>
       </c>
-      <c r="F5" s="25" t="n"/>
+      <c r="F5" s="26" t="n"/>
       <c r="G5" s="23" t="inlineStr">
         <is>
           <t>Storage integration needs</t>
@@ -4088,33 +4119,33 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="10" t="inlineStr">
+      <c r="A6" s="25" t="inlineStr">
         <is>
           <t>TECH-005</t>
         </is>
       </c>
-      <c r="B6" s="10" t="inlineStr">
+      <c r="B6" s="25" t="inlineStr">
         <is>
           <t>Technical Requirements</t>
         </is>
       </c>
-      <c r="C6" s="10" t="inlineStr">
+      <c r="C6" s="25" t="inlineStr">
         <is>
           <t>API Requirements</t>
         </is>
       </c>
-      <c r="D6" s="10" t="inlineStr">
+      <c r="D6" s="25" t="inlineStr">
         <is>
           <t>Do you need real-time or batch document processing?</t>
         </is>
       </c>
-      <c r="E6" s="10" t="inlineStr">
+      <c r="E6" s="25" t="inlineStr">
         <is>
           <t>Options: Real-time processing, Batch processing, Both options</t>
         </is>
       </c>
-      <c r="F6" s="25" t="n"/>
-      <c r="G6" s="10" t="inlineStr">
+      <c r="F6" s="26" t="n"/>
+      <c r="G6" s="25" t="inlineStr">
         <is>
           <t>Processing mode requirements</t>
         </is>
@@ -4146,7 +4177,7 @@
           <t>Common integrations: REST APIs, Webhooks, File upload endpoints, Email integration, FTP integration</t>
         </is>
       </c>
-      <c r="F7" s="25" t="n"/>
+      <c r="F7" s="26" t="n"/>
       <c r="G7" s="23" t="inlineStr">
         <is>
           <t>API integration needs</t>
@@ -4154,29 +4185,29 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="10" t="inlineStr">
+      <c r="A8" s="25" t="inlineStr">
         <is>
           <t>TECH-007</t>
         </is>
       </c>
-      <c r="B8" s="10" t="inlineStr">
+      <c r="B8" s="25" t="inlineStr">
         <is>
           <t>Technical Requirements</t>
         </is>
       </c>
-      <c r="C8" s="10" t="inlineStr">
+      <c r="C8" s="25" t="inlineStr">
         <is>
           <t>Performance</t>
         </is>
       </c>
-      <c r="D8" s="10" t="inlineStr">
+      <c r="D8" s="25" t="inlineStr">
         <is>
           <t>What are your document processing speed requirements?</t>
         </is>
       </c>
-      <c r="E8" s="10" t="n"/>
-      <c r="F8" s="25" t="n"/>
-      <c r="G8" s="10" t="inlineStr">
+      <c r="E8" s="25" t="n"/>
+      <c r="F8" s="26" t="n"/>
+      <c r="G8" s="25" t="inlineStr">
         <is>
           <t>Performance expectations</t>
         </is>
@@ -4208,7 +4239,7 @@
           <t>Common targets: 95%+, 98%+, 99%+, 99.5%+</t>
         </is>
       </c>
-      <c r="F9" s="25" t="n"/>
+      <c r="F9" s="26" t="n"/>
       <c r="G9" s="23" t="inlineStr">
         <is>
           <t>Accuracy requirements</t>
@@ -4216,33 +4247,33 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="inlineStr">
+      <c r="A10" s="25" t="inlineStr">
         <is>
           <t>TECH-009</t>
         </is>
       </c>
-      <c r="B10" s="10" t="inlineStr">
+      <c r="B10" s="25" t="inlineStr">
         <is>
           <t>Technical Requirements</t>
         </is>
       </c>
-      <c r="C10" s="10" t="inlineStr">
+      <c r="C10" s="25" t="inlineStr">
         <is>
           <t>Security</t>
         </is>
       </c>
-      <c r="D10" s="10" t="inlineStr">
+      <c r="D10" s="25" t="inlineStr">
         <is>
           <t>What security requirements apply to document processing?</t>
         </is>
       </c>
-      <c r="E10" s="10" t="inlineStr">
+      <c r="E10" s="25" t="inlineStr">
         <is>
           <t>Common requirements: Encryption at rest, Encryption in transit, Access controls, Audit logging, Data masking</t>
         </is>
       </c>
-      <c r="F10" s="25" t="n"/>
-      <c r="G10" s="10" t="inlineStr">
+      <c r="F10" s="26" t="n"/>
+      <c r="G10" s="25" t="inlineStr">
         <is>
           <t>Security controls needed</t>
         </is>
@@ -4274,7 +4305,7 @@
           <t>Common standards: SOC 2, ISO 27001, HIPAA, PCI DSS, GDPR, FedRAMP, None</t>
         </is>
       </c>
-      <c r="F11" s="25" t="n"/>
+      <c r="F11" s="26" t="n"/>
       <c r="G11" s="23" t="inlineStr">
         <is>
           <t>Compliance requirements</t>
@@ -4282,33 +4313,33 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="inlineStr">
+      <c r="A12" s="25" t="inlineStr">
         <is>
           <t>TECH-011</t>
         </is>
       </c>
-      <c r="B12" s="10" t="inlineStr">
+      <c r="B12" s="25" t="inlineStr">
         <is>
           <t>Technical Requirements</t>
         </is>
       </c>
-      <c r="C12" s="10" t="inlineStr">
+      <c r="C12" s="25" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
       </c>
-      <c r="D12" s="10" t="inlineStr">
+      <c r="D12" s="25" t="inlineStr">
         <is>
           <t>What sensitive data types are present in your documents?</t>
         </is>
       </c>
-      <c r="E12" s="10" t="inlineStr">
+      <c r="E12" s="25" t="inlineStr">
         <is>
           <t>Sensitive data types: PII, PHI, Financial data, Credit card numbers, SSNs, Other sensitive data, No sensitive data</t>
         </is>
       </c>
-      <c r="F12" s="25" t="n"/>
-      <c r="G12" s="10" t="inlineStr">
+      <c r="F12" s="26" t="n"/>
+      <c r="G12" s="25" t="inlineStr">
         <is>
           <t>Data protection requirements</t>
         </is>
@@ -4336,7 +4367,7 @@
         </is>
       </c>
       <c r="E13" s="23" t="n"/>
-      <c r="F13" s="25" t="n"/>
+      <c r="F13" s="26" t="n"/>
       <c r="G13" s="23" t="inlineStr">
         <is>
           <t>Data lifecycle management</t>
@@ -4344,33 +4375,33 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="10" t="inlineStr">
+      <c r="A14" s="25" t="inlineStr">
         <is>
           <t>TECH-013</t>
         </is>
       </c>
-      <c r="B14" s="10" t="inlineStr">
+      <c r="B14" s="25" t="inlineStr">
         <is>
           <t>Technical Requirements</t>
         </is>
       </c>
-      <c r="C14" s="10" t="inlineStr">
+      <c r="C14" s="25" t="inlineStr">
         <is>
           <t>Availability</t>
         </is>
       </c>
-      <c r="D14" s="10" t="inlineStr">
+      <c r="D14" s="25" t="inlineStr">
         <is>
           <t>What uptime requirements do you have for document processing?</t>
         </is>
       </c>
-      <c r="E14" s="10" t="inlineStr">
+      <c r="E14" s="25" t="inlineStr">
         <is>
           <t>Common targets: 99%, 99.5%, 99.9%, 99.95%, 99.99%</t>
         </is>
       </c>
-      <c r="F14" s="25" t="n"/>
-      <c r="G14" s="10" t="inlineStr">
+      <c r="F14" s="26" t="n"/>
+      <c r="G14" s="25" t="inlineStr">
         <is>
           <t>SLA requirements</t>
         </is>
@@ -4405,7 +4436,7 @@
     <col width="30" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="32" customHeight="1">
+    <row r="1" ht="30" customHeight="1">
       <c r="A1" s="22" t="inlineStr">
         <is>
           <t>Question ID</t>
@@ -4443,33 +4474,33 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="inlineStr">
+      <c r="A2" s="25" t="inlineStr">
         <is>
           <t>AI-001</t>
         </is>
       </c>
-      <c r="B2" s="10" t="inlineStr">
+      <c r="B2" s="25" t="inlineStr">
         <is>
           <t>AI/ML Requirements</t>
         </is>
       </c>
-      <c r="C2" s="10" t="inlineStr">
+      <c r="C2" s="25" t="inlineStr">
         <is>
           <t>Model Needs</t>
         </is>
       </c>
-      <c r="D2" s="10" t="inlineStr">
+      <c r="D2" s="25" t="inlineStr">
         <is>
           <t>Do you need custom ML models or will AWS pre-built services suffice?</t>
         </is>
       </c>
-      <c r="E2" s="10" t="inlineStr">
+      <c r="E2" s="25" t="inlineStr">
         <is>
           <t>Options: AWS Textract only, AWS Comprehend only, Custom classification models, Custom extraction models, Combination approach</t>
         </is>
       </c>
-      <c r="F2" s="25" t="n"/>
-      <c r="G2" s="10" t="inlineStr">
+      <c r="F2" s="26" t="n"/>
+      <c r="G2" s="25" t="inlineStr">
         <is>
           <t>Model complexity requirements</t>
         </is>
@@ -4501,7 +4532,7 @@
           <t>Options: Yes - substantial dataset, Yes - limited dataset, No - need data labeling, Unsure</t>
         </is>
       </c>
-      <c r="F3" s="25" t="n"/>
+      <c r="F3" s="26" t="n"/>
       <c r="G3" s="23" t="inlineStr">
         <is>
           <t>Training data availability</t>
@@ -4509,33 +4540,33 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="inlineStr">
+      <c r="A4" s="25" t="inlineStr">
         <is>
           <t>AI-003</t>
         </is>
       </c>
-      <c r="B4" s="10" t="inlineStr">
+      <c r="B4" s="25" t="inlineStr">
         <is>
           <t>AI/ML Requirements</t>
         </is>
       </c>
-      <c r="C4" s="10" t="inlineStr">
+      <c r="C4" s="25" t="inlineStr">
         <is>
           <t>Accuracy Improvement</t>
         </is>
       </c>
-      <c r="D4" s="10" t="inlineStr">
+      <c r="D4" s="25" t="inlineStr">
         <is>
           <t>How will you handle cases where extraction accuracy is low?</t>
         </is>
       </c>
-      <c r="E4" s="10" t="inlineStr">
+      <c r="E4" s="25" t="inlineStr">
         <is>
           <t>Options: Human review workflow (A2I), Confidence scoring, Automated rejection, Manual correction interface</t>
         </is>
       </c>
-      <c r="F4" s="25" t="n"/>
-      <c r="G4" s="10" t="inlineStr">
+      <c r="F4" s="26" t="n"/>
+      <c r="G4" s="25" t="inlineStr">
         <is>
           <t>Quality assurance process</t>
         </is>
@@ -4567,7 +4598,7 @@
           <t>Options: Never, Quarterly, Monthly, As needed, Continuously</t>
         </is>
       </c>
-      <c r="F5" s="25" t="n"/>
+      <c r="F5" s="26" t="n"/>
       <c r="G5" s="23" t="inlineStr">
         <is>
           <t>Model maintenance expectations</t>
@@ -4603,7 +4634,7 @@
     <col width="30" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="32" customHeight="1">
+    <row r="1" ht="30" customHeight="1">
       <c r="A1" s="22" t="inlineStr">
         <is>
           <t>Question ID</t>
@@ -4641,29 +4672,29 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="inlineStr">
+      <c r="A2" s="25" t="inlineStr">
         <is>
           <t>ORG-001</t>
         </is>
       </c>
-      <c r="B2" s="10" t="inlineStr">
+      <c r="B2" s="25" t="inlineStr">
         <is>
           <t>Organizational</t>
         </is>
       </c>
-      <c r="C2" s="10" t="inlineStr">
+      <c r="C2" s="25" t="inlineStr">
         <is>
           <t>Resources</t>
         </is>
       </c>
-      <c r="D2" s="10" t="inlineStr">
+      <c r="D2" s="25" t="inlineStr">
         <is>
           <t>Who will be the technical lead for this IDP project?</t>
         </is>
       </c>
-      <c r="E2" s="10" t="n"/>
-      <c r="F2" s="25" t="n"/>
-      <c r="G2" s="10" t="inlineStr">
+      <c r="E2" s="25" t="n"/>
+      <c r="F2" s="26" t="n"/>
+      <c r="G2" s="25" t="inlineStr">
         <is>
           <t>Technical ownership</t>
         </is>
@@ -4691,7 +4722,7 @@
         </is>
       </c>
       <c r="E3" s="23" t="n"/>
-      <c r="F3" s="25" t="n"/>
+      <c r="F3" s="26" t="n"/>
       <c r="G3" s="23" t="inlineStr">
         <is>
           <t>Team availability</t>
@@ -4699,33 +4730,33 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="inlineStr">
+      <c r="A4" s="25" t="inlineStr">
         <is>
           <t>ORG-003</t>
         </is>
       </c>
-      <c r="B4" s="10" t="inlineStr">
+      <c r="B4" s="25" t="inlineStr">
         <is>
           <t>Organizational</t>
         </is>
       </c>
-      <c r="C4" s="10" t="inlineStr">
+      <c r="C4" s="25" t="inlineStr">
         <is>
           <t>Resources</t>
         </is>
       </c>
-      <c r="D4" s="10" t="inlineStr">
+      <c r="D4" s="25" t="inlineStr">
         <is>
           <t>What is your team's experience with AWS AI/ML services?</t>
         </is>
       </c>
-      <c r="E4" s="10" t="inlineStr">
+      <c r="E4" s="25" t="inlineStr">
         <is>
           <t>Experience levels: No experience, Basic knowledge, Intermediate, Advanced, Expert</t>
         </is>
       </c>
-      <c r="F4" s="25" t="n"/>
-      <c r="G4" s="10" t="inlineStr">
+      <c r="F4" s="26" t="n"/>
+      <c r="G4" s="25" t="inlineStr">
         <is>
           <t>Training needs assessment</t>
         </is>
@@ -4753,7 +4784,7 @@
         </is>
       </c>
       <c r="E5" s="23" t="n"/>
-      <c r="F5" s="25" t="n"/>
+      <c r="F5" s="26" t="n"/>
       <c r="G5" s="23" t="inlineStr">
         <is>
           <t>Change management approach</t>
@@ -4761,29 +4792,29 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="10" t="inlineStr">
+      <c r="A6" s="25" t="inlineStr">
         <is>
           <t>ORG-005</t>
         </is>
       </c>
-      <c r="B6" s="10" t="inlineStr">
+      <c r="B6" s="25" t="inlineStr">
         <is>
           <t>Organizational</t>
         </is>
       </c>
-      <c r="C6" s="10" t="inlineStr">
+      <c r="C6" s="25" t="inlineStr">
         <is>
           <t>Change Management</t>
         </is>
       </c>
-      <c r="D6" s="10" t="inlineStr">
+      <c r="D6" s="25" t="inlineStr">
         <is>
           <t>What training will be needed for end users?</t>
         </is>
       </c>
-      <c r="E6" s="10" t="n"/>
-      <c r="F6" s="25" t="n"/>
-      <c r="G6" s="10" t="inlineStr">
+      <c r="E6" s="25" t="n"/>
+      <c r="F6" s="26" t="n"/>
+      <c r="G6" s="25" t="inlineStr">
         <is>
           <t>Training requirements</t>
         </is>
@@ -4811,7 +4842,7 @@
         </is>
       </c>
       <c r="E7" s="23" t="n"/>
-      <c r="F7" s="25" t="n"/>
+      <c r="F7" s="26" t="n"/>
       <c r="G7" s="23" t="inlineStr">
         <is>
           <t>Change approval process</t>
@@ -4847,7 +4878,7 @@
     <col width="30" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="32" customHeight="1">
+    <row r="1" ht="30" customHeight="1">
       <c r="A1" s="22" t="inlineStr">
         <is>
           <t>Question ID</t>
@@ -4885,29 +4916,29 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="inlineStr">
+      <c r="A2" s="25" t="inlineStr">
         <is>
           <t>WORKFLOW-001</t>
         </is>
       </c>
-      <c r="B2" s="10" t="inlineStr">
+      <c r="B2" s="25" t="inlineStr">
         <is>
           <t>Workflow Requirements</t>
         </is>
       </c>
-      <c r="C2" s="10" t="inlineStr">
+      <c r="C2" s="25" t="inlineStr">
         <is>
           <t>Process Flow</t>
         </is>
       </c>
-      <c r="D2" s="10" t="inlineStr">
+      <c r="D2" s="25" t="inlineStr">
         <is>
           <t>What happens to documents after data extraction?</t>
         </is>
       </c>
-      <c r="E2" s="10" t="n"/>
-      <c r="F2" s="25" t="n"/>
-      <c r="G2" s="10" t="inlineStr">
+      <c r="E2" s="25" t="n"/>
+      <c r="F2" s="26" t="n"/>
+      <c r="G2" s="25" t="inlineStr">
         <is>
           <t>Downstream processing requirements</t>
         </is>
@@ -4935,7 +4966,7 @@
         </is>
       </c>
       <c r="E3" s="23" t="n"/>
-      <c r="F3" s="25" t="n"/>
+      <c r="F3" s="26" t="n"/>
       <c r="G3" s="23" t="inlineStr">
         <is>
           <t>Error handling requirements</t>
@@ -4943,33 +4974,33 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="inlineStr">
+      <c r="A4" s="25" t="inlineStr">
         <is>
           <t>WORKFLOW-003</t>
         </is>
       </c>
-      <c r="B4" s="10" t="inlineStr">
+      <c r="B4" s="25" t="inlineStr">
         <is>
           <t>Workflow Requirements</t>
         </is>
       </c>
-      <c r="C4" s="10" t="inlineStr">
+      <c r="C4" s="25" t="inlineStr">
         <is>
           <t>Process Flow</t>
         </is>
       </c>
-      <c r="D4" s="10" t="inlineStr">
+      <c r="D4" s="25" t="inlineStr">
         <is>
           <t>Do you need human-in-the-loop review capabilities?</t>
         </is>
       </c>
-      <c r="E4" s="10" t="inlineStr">
+      <c r="E4" s="25" t="inlineStr">
         <is>
           <t>Options: Always required, Only for low confidence, Only for exceptions, Never needed</t>
         </is>
       </c>
-      <c r="F4" s="25" t="n"/>
-      <c r="G4" s="10" t="inlineStr">
+      <c r="F4" s="26" t="n"/>
+      <c r="G4" s="25" t="inlineStr">
         <is>
           <t>Human review requirements (Amazon A2I)</t>
         </is>
@@ -4997,7 +5028,7 @@
         </is>
       </c>
       <c r="E5" s="23" t="n"/>
-      <c r="F5" s="25" t="n"/>
+      <c r="F5" s="26" t="n"/>
       <c r="G5" s="23" t="inlineStr">
         <is>
           <t>Notification requirements</t>

</xml_diff>